<commit_message>
LGX Cable buddy stl
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie BOM RC-08.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie BOM RC-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="388" documentId="11_90E8A2594C63906364F20E90CDD1628CCD4781EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{872306E5-997C-4E46-BA8E-26A758D5D70D}"/>
+  <xr:revisionPtr revIDLastSave="395" documentId="11_90E8A2594C63906364F20E90CDD1628CCD4781EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B420C59B-36A5-4A09-9736-9F8CA0A43259}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3409,12 +3409,12 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:P1"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
     <col min="2" max="2" width="13.453125" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.1796875" customWidth="1"/>
@@ -3425,11 +3425,11 @@
     <col min="9" max="9" width="13.1796875" customWidth="1"/>
     <col min="10" max="10" width="14.81640625" customWidth="1"/>
     <col min="11" max="11" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26953125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8.54296875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" customWidth="1"/>
+    <col min="14" max="14" width="8.54296875" customWidth="1"/>
     <col min="15" max="15" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.54296875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" customWidth="1"/>
     <col min="17" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>